<commit_message>
Update sql implementantion and bug sever-split file
</commit_message>
<xml_diff>
--- a/resources/count_implementation.xlsx
+++ b/resources/count_implementation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,22 +461,22 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>mybatis</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Hibernate</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>jOOQ</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>JPA</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Mybatis</t>
         </is>
       </c>
     </row>
@@ -495,154 +495,187 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>60</v>
+        <v>0.01224739742804654</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>0.01000204123290467</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.0004082465809348847</v>
       </c>
       <c r="H2" t="n">
-        <v>317</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>50</v>
+        <v>0.01285976729944887</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>skywalking</t>
+          <t>che</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>monitoring</t>
+          <t>software development</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.01536643026004728</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.0007880220646178094</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0.002758077226162333</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>0.04137115839243499</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>storm</t>
+          <t>pinpoint</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>hpc</t>
+          <t>monitoring</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0.004785863296109952</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.005276721070069947</v>
       </c>
       <c r="G4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>che</t>
+          <t>skywalking</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>software development</t>
+          <t>monitoring</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.0003865481252415926</v>
       </c>
       <c r="H5" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>9</v>
+        <v>0.0003865481252415926</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>pinpoint</t>
+          <t>wildfly</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>monitoring</t>
+          <t>infrastructure management</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.002059805383905107</v>
       </c>
       <c r="D6" t="n">
-        <v>40</v>
+        <v>0.0002130833155763904</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.01207472121599545</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.01640741529938206</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>43</v>
+        <v>0.03821294126003268</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>storm</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>hpc</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0005885815185403178</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0008828722778104767</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.001765744555620953</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IgnoreCase, count implementation, and extract
</commit_message>
<xml_diff>
--- a/resources/count_implementation.xlsx
+++ b/resources/count_implementation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>JPA</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Number total of files</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -495,22 +500,28 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01224739742804654</v>
+        <v>60</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01000204123290467</v>
+        <v>49</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0004082465809348847</v>
+        <v>2</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.01285976729944887</v>
+        <v>63</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    4899
+</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -525,16 +536,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.01536643026004728</v>
+        <v>39</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0007880220646178094</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.002758077226162333</v>
+        <v>7</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -543,7 +554,13 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.04137115839243499</v>
+        <v>105</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    2538
+</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -561,13 +578,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.004785863296109952</v>
+        <v>39</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.005276721070069947</v>
+        <v>43</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -577,6 +594,12 @@
       </c>
       <c r="I4" t="n">
         <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    8149
+</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -603,13 +626,19 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0003865481252415926</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0003865481252415926</v>
+        <v>1</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    2587
+</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -624,25 +653,31 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.002059805383905107</v>
+        <v>29</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0002130833155763904</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01207472121599545</v>
+        <v>170</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01640741529938206</v>
+        <v>231</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.03821294126003268</v>
+        <v>538</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   14079
+</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -660,22 +695,28 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0005885815185403178</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0008828722778104767</v>
+        <v>3</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.001765744555620953</v>
+        <v>6</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    3398
+</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Results RQ2 and RQ3
</commit_message>
<xml_diff>
--- a/resources/count_implementation.xlsx
+++ b/resources/count_implementation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,28 +488,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CoreNLP</t>
+          <t>Activiti</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Artificial Intelligence</t>
+          <t>Enterprise Resource Planning</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>60</v>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>15</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
+        <v>50</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2</v>
+      </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    3006
+          <t xml:space="preserve">    5151
 </t>
         </is>
       </c>
@@ -517,12 +521,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>strimzi-kafka-operator</t>
+          <t>lottie-android</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Infrastructure Management</t>
+          <t>Game</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -534,7 +538,7 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t xml:space="preserve">    2665
+          <t xml:space="preserve">    1273
 </t>
         </is>
       </c>
@@ -542,7 +546,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>swagger-core</t>
+          <t>spring-cloud-alibaba</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -553,13 +557,17 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1138
+          <t xml:space="preserve">     841
 </t>
         </is>
       </c>
@@ -567,24 +575,28 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>syncthing-android</t>
+          <t>nacos</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>File Management</t>
+          <t>Infrastructure Management</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>14</v>
+      </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t xml:space="preserve">     392
+          <t xml:space="preserve">    2935
 </t>
         </is>
       </c>
@@ -592,7 +604,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>synthea</t>
+          <t>fastjson</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -601,17 +613,21 @@
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>11</v>
+      </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1488
+          <t xml:space="preserve">    3249
 </t>
         </is>
       </c>
@@ -619,28 +635,24 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AmazeFileManager</t>
+          <t>aliyun-openapi-java-sdk</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>File Management</t>
+          <t>Infrastructure Management</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>11</v>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
-        <v>11</v>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1298
+          <t xml:space="preserve">   59971
 </t>
         </is>
       </c>
@@ -648,24 +660,26 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>teammates</t>
+          <t>alluxio</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Collaboration</t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">     206
+          <t xml:space="preserve">    4092
 </t>
         </is>
       </c>
@@ -673,28 +687,24 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NewPipe</t>
+          <t>FXGL</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Media</t>
+          <t>Game</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>6</v>
-      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="n">
-        <v>12</v>
-      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t xml:space="preserve">    3149
+          <t xml:space="preserve">    1370
 </t>
         </is>
       </c>
@@ -702,36 +712,24 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>FrameworkBenchmarks</t>
+          <t>android-beacon-library</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>15</v>
-      </c>
-      <c r="D10" t="n">
-        <v>2</v>
-      </c>
+          <t>Network</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>4</v>
-      </c>
-      <c r="G10" t="n">
-        <v>30</v>
-      </c>
-      <c r="H10" t="n">
-        <v>9</v>
-      </c>
-      <c r="I10" t="n">
-        <v>79</v>
-      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
-          <t xml:space="preserve">    7405
+          <t xml:space="preserve">     148
 </t>
         </is>
       </c>
@@ -739,7 +737,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>testcontainers-java</t>
+          <t>streamex</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -748,19 +746,15 @@
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
-        <v>2</v>
-      </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1338
+          <t xml:space="preserve">     129
 </t>
         </is>
       </c>
@@ -768,30 +762,26 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>onedev</t>
+          <t>AntennaPod</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Collaboration</t>
+          <t>Media</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="n">
-        <v>10</v>
-      </c>
-      <c r="G12" t="n">
-        <v>154</v>
-      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
-        <v>163</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">    5003
+          <t xml:space="preserve">    1157
 </t>
         </is>
       </c>
@@ -799,32 +789,26 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>thingsboard</t>
+          <t>antlr4</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Artificial Intelligence </t>
+          <t>Software Development</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="n">
-        <v>8</v>
-      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>12</v>
-      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
-        <v>73</v>
-      </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve">    8179
+          <t xml:space="preserve">    2292
 </t>
         </is>
       </c>
@@ -832,26 +816,24 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>tlaplus</t>
+          <t>AnySoftKeyboard</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Program Analysis</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="n">
-        <v>3</v>
-      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t xml:space="preserve">    5327
+          <t xml:space="preserve">    6713
 </t>
         </is>
       </c>
@@ -859,28 +841,24 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ArchUnit</t>
+          <t>rocketmq</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Program Analysis</t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
-        <v>2</v>
-      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="n">
-        <v>25</v>
-      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1665
+          <t xml:space="preserve">    2533
 </t>
         </is>
       </c>
@@ -888,26 +866,28 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>traccar</t>
+          <t>hudi</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Network</t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>7</v>
-      </c>
-      <c r="G16" t="inlineStr"/>
+        <v>18</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2</v>
+      </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1517
+          <t xml:space="preserve">    4165
 </t>
         </is>
       </c>
@@ -915,7 +895,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>trino</t>
+          <t>iceberg</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -927,14 +907,14 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
-          <t xml:space="preserve">   14733
+          <t xml:space="preserve">    4536
 </t>
         </is>
       </c>
@@ -942,24 +922,34 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>java-tron</t>
+          <t>servicecomb-pack</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Cryptocurrency</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
+          <t>Enterprise Resource Planning</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>27</v>
+      </c>
+      <c r="D18" t="n">
+        <v>32</v>
+      </c>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>12</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3</v>
+      </c>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>13</v>
+      </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1417
+          <t xml:space="preserve">     979
 </t>
         </is>
       </c>
@@ -967,26 +957,32 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Twitter4J</t>
+          <t>shiro</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Media</t>
+          <t>Security</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>6</v>
+      </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>3</v>
+      </c>
+      <c r="G19" t="n">
+        <v>7</v>
+      </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">     533
+          <t xml:space="preserve">    1260
 </t>
         </is>
       </c>
@@ -994,12 +990,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>afwall</t>
+          <t>opennlp</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Security</t>
+          <t xml:space="preserve">Artificial Intelligence </t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -1011,7 +1007,7 @@
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t xml:space="preserve">     526
+          <t xml:space="preserve">    1372
 </t>
         </is>
       </c>
@@ -1019,28 +1015,28 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>fitnesse</t>
+          <t>zookeeper</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Program Analysis</t>
+          <t>Infrastructure Management</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t xml:space="preserve">    2818
+          <t xml:space="preserve">    1503
 </t>
         </is>
       </c>
@@ -1048,24 +1044,28 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>undertow</t>
+          <t>avro</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Infrastructure Management</t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>40</v>
+      </c>
+      <c r="G22" t="n">
+        <v>9</v>
+      </c>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1551
+          <t xml:space="preserve">    2275
 </t>
         </is>
       </c>
@@ -1073,26 +1073,28 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>UniversalMediaServer</t>
+          <t>shardingsphere-elasticjob</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Media</t>
+          <t>Infrastructure Management</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="n">
+        <v>29</v>
+      </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
-          <t xml:space="preserve">    2472
+          <t xml:space="preserve">    1084
 </t>
         </is>
       </c>
@@ -1100,34 +1102,26 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>framework</t>
+          <t>bookkeeper</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Software Development</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>2</v>
-      </c>
-      <c r="D24" t="n">
-        <v>3</v>
-      </c>
+          <t>Data Management</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="n">
-        <v>6</v>
-      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="n">
-        <v>3</v>
-      </c>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr">
         <is>
-          <t xml:space="preserve">   10118
+          <t xml:space="preserve">    3268
 </t>
         </is>
       </c>
@@ -1135,26 +1129,24 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>validator</t>
+          <t>curator</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Software Development</t>
+          <t>Infrastructure Management</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
-      <c r="F25" t="n">
-        <v>11</v>
-      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
-          <t xml:space="preserve">     721
+          <t xml:space="preserve">     766
 </t>
         </is>
       </c>
@@ -1162,7 +1154,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>vavr</t>
+          <t>netbeans</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1170,16 +1162,26 @@
           <t>Software Development</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+      <c r="C26" t="n">
+        <v>95</v>
+      </c>
+      <c r="D26" t="n">
+        <v>39</v>
+      </c>
       <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+      <c r="F26" t="n">
+        <v>460</v>
+      </c>
+      <c r="G26" t="n">
+        <v>234</v>
+      </c>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="n">
+        <v>267</v>
+      </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">     333
+          <t xml:space="preserve">   91104
 </t>
         </is>
       </c>
@@ -1187,30 +1189,26 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>modeldb</t>
+          <t>nutch</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Artificial Intelligence </t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
-        <v>4</v>
-      </c>
-      <c r="G27" t="n">
-        <v>54</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
-      <c r="I27" t="n">
-        <v>57</v>
-      </c>
+      <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
-          <t xml:space="preserve">    4314
+          <t xml:space="preserve">    1101
 </t>
         </is>
       </c>
@@ -1218,30 +1216,30 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>vespa</t>
+          <t>servicecomb-java-chassis</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Data Management</t>
+          <t>Infrastructure Management</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>7</v>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="G28" t="n">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="H28" t="inlineStr"/>
-      <c r="I28" t="n">
-        <v>2</v>
-      </c>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve">   22041
+          <t xml:space="preserve">    3215
 </t>
         </is>
       </c>
@@ -1249,26 +1247,24 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>fastutil</t>
+          <t>httpcomponents-client</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Data Management</t>
+          <t>Network</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
-      <c r="F29" t="n">
-        <v>1</v>
-      </c>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr">
         <is>
-          <t xml:space="preserve">     277
+          <t xml:space="preserve">     829
 </t>
         </is>
       </c>
@@ -1276,28 +1272,26 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Saturn</t>
+          <t>calcite</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Automation</t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
-      <c r="D30" t="n">
-        <v>6</v>
-      </c>
+      <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
         <is>
-          <t xml:space="preserve">     882
+          <t xml:space="preserve">    2947
 </t>
         </is>
       </c>
@@ -1305,26 +1299,30 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>flexmark-java</t>
+          <t>dubbo</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Software Development</t>
+          <t>Infrastructure Management</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>77</v>
+      </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G31" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5</v>
+      </c>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
-          <t xml:space="preserve">    2981
+          <t xml:space="preserve">    4667
 </t>
         </is>
       </c>
@@ -1332,26 +1330,30 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>epubcheck</t>
+          <t>drill</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Program Analysis</t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
-        <v>36</v>
-      </c>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" t="n">
+        <v>15</v>
+      </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
-          <t xml:space="preserve">    3695
+          <t xml:space="preserve">    6529
 </t>
         </is>
       </c>
@@ -1359,26 +1361,26 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>dynmap</t>
+          <t>pulsar</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Game</t>
+          <t>Network</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
-      <c r="F33" t="n">
-        <v>1</v>
-      </c>
-      <c r="G33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="n">
+        <v>28</v>
+      </c>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr">
         <is>
-          <t xml:space="preserve">    4569
+          <t xml:space="preserve">    5233
 </t>
         </is>
       </c>
@@ -1386,34 +1388,26 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>wildfly</t>
+          <t>zeppelin</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Infrastructure Management</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>15</v>
-      </c>
-      <c r="D34" t="n">
-        <v>1</v>
-      </c>
+          <t>Data Management</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
-        <v>68</v>
-      </c>
-      <c r="G34" t="n">
-        <v>170</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
-      <c r="I34" t="n">
-        <v>416</v>
-      </c>
+      <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr">
         <is>
-          <t xml:space="preserve">   13493
+          <t xml:space="preserve">    2410
 </t>
         </is>
       </c>
@@ -1421,26 +1415,24 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Universal-G-Code-Sender</t>
+          <t>iotdb</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Automation</t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
-      <c r="F35" t="n">
-        <v>6</v>
-      </c>
+      <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
-          <t xml:space="preserve">    2921
+          <t xml:space="preserve">    6092
 </t>
         </is>
       </c>
@@ -1448,28 +1440,32 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>xxl-job</t>
+          <t>skywalking</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Automation</t>
+          <t>Monitoring</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
-        <v>20</v>
-      </c>
-      <c r="G36" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
+      </c>
       <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
+      <c r="I36" t="n">
+        <v>2</v>
+      </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t xml:space="preserve">     287
+          <t xml:space="preserve">    3833
 </t>
         </is>
       </c>
@@ -1477,26 +1473,28 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>yacy_search_server</t>
+          <t>tika</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Infrastructure Management</t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
         <is>
-          <t xml:space="preserve">    1888
+          <t xml:space="preserve">    3682
 </t>
         </is>
       </c>
@@ -1504,26 +1502,30 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>zaproxy</t>
+          <t>nifi</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Security</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr"/>
+          <t>Data Management</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
         <v>2</v>
       </c>
-      <c r="G38" t="inlineStr"/>
+      <c r="G38" t="n">
+        <v>1</v>
+      </c>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr">
         <is>
-          <t xml:space="preserve">    2269
+          <t xml:space="preserve">   12754
 </t>
         </is>
       </c>
@@ -1531,24 +1533,30 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>maxwell</t>
+          <t>commons-lang</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Data Management</t>
+          <t>Software Development</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1</v>
+      </c>
       <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
+      <c r="I39" t="n">
+        <v>2</v>
+      </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t xml:space="preserve">     490
+          <t xml:space="preserve">     583
 </t>
         </is>
       </c>
@@ -1556,24 +1564,26 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>jeromq</t>
+          <t>gobblin</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Infrastructure Management</t>
+          <t>Data Management</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
+      <c r="F40" t="n">
+        <v>1</v>
+      </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t xml:space="preserve">     471
+          <t xml:space="preserve">    4496
 </t>
         </is>
       </c>
@@ -1581,7 +1591,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>zxing</t>
+          <t>struts</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1590,17 +1600,866 @@
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
+      <c r="D41" t="n">
+        <v>3</v>
+      </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="n">
-        <v>5</v>
-      </c>
-      <c r="G41" t="inlineStr"/>
+        <v>63</v>
+      </c>
+      <c r="G41" t="n">
+        <v>10</v>
+      </c>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr">
         <is>
-          <t xml:space="preserve">    3768
+          <t xml:space="preserve">    3436
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>kafka</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Infrastructure Management</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="n">
+        <v>4</v>
+      </c>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="n">
+        <v>1</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    6523
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>geode</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Data Management</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="n">
+        <v>6</v>
+      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="n">
+        <v>64</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3</v>
+      </c>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   10414
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>pdfbox</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    1878
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>storm</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Data Management</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="n">
+        <v>3</v>
+      </c>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    3093
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>activemq</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="n">
+        <v>225</v>
+      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="n">
+        <v>10</v>
+      </c>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="n">
+        <v>56</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    5322
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>maven</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="n">
+        <v>13</v>
+      </c>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    2106
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>poi</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="n">
+        <v>3</v>
+      </c>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    5481
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>logging-log4j2</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="n">
+        <v>4</v>
+      </c>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="n">
+        <v>3</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    2232
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>hive</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Data Management</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="n">
+        <v>13</v>
+      </c>
+      <c r="G50" t="n">
+        <v>2</v>
+      </c>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   21272
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>groovy</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>2</v>
+      </c>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="n">
+        <v>2</v>
+      </c>
+      <c r="G51" t="n">
+        <v>4</v>
+      </c>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="n">
+        <v>2</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    5013
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>jmeter</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Automation</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="n">
+        <v>6</v>
+      </c>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    3978
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>tinkerpop</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Data Management</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="n">
+        <v>14</v>
+      </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    3744
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>flink</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Data Management</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="n">
+        <v>1</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   24422
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>tomcat</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Infrastructure Management</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="n">
+        <v>5</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="n">
+        <v>4</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    4514
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>hadoop</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Data Management</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    7510
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>beam</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Data Management</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" t="n">
+        <v>14</v>
+      </c>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   14546
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ambari</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Infrastructure Management</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>50</v>
+      </c>
+      <c r="D58" t="n">
+        <v>8</v>
+      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="n">
+        <v>43</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="n">
+        <v>269</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   10718
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>camel</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="n">
+        <v>1280</v>
+      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="n">
+        <v>19</v>
+      </c>
+      <c r="G59" t="n">
+        <v>9</v>
+      </c>
+      <c r="H59" t="n">
+        <v>12</v>
+      </c>
+      <c r="I59" t="n">
+        <v>49</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   33526
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>cas</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Security</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>7</v>
+      </c>
+      <c r="D60" t="n">
+        <v>9</v>
+      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="n">
+        <v>36</v>
+      </c>
+      <c r="G60" t="n">
+        <v>30</v>
+      </c>
+      <c r="H60" t="n">
+        <v>267</v>
+      </c>
+      <c r="I60" t="n">
+        <v>82</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   11034
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>AsciidocFX</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Media</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="n">
+        <v>5</v>
+      </c>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    1643
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>async-http-client</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     370
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>commafeed</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Collaboration</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="n">
+        <v>8</v>
+      </c>
+      <c r="G63" t="n">
+        <v>7</v>
+      </c>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="n">
+        <v>21</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     373
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>atmosphere</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     385
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>simplenote-android</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Personal Management</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     724
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>aws-sdk-java-v2</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Infrastructure Management</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    9545
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>AxonFramework</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Infrastructure Management</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="n">
+        <v>4</v>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="n">
+        <v>11</v>
+      </c>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="n">
+        <v>108</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    2219
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>azkaban</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Automation</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="n">
+        <v>9</v>
+      </c>
+      <c r="G68" t="n">
+        <v>1</v>
+      </c>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    1894
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>bazel</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Software Development</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="n">
+        <v>4</v>
+      </c>
+      <c r="G69" t="n">
+        <v>7</v>
+      </c>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    8413
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>bc-java</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Security</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="n">
+        <v>3</v>
+      </c>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    8675
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
export complete results to xlsx
</commit_message>
<xml_diff>
--- a/resources/count_implementation.xlsx
+++ b/resources/count_implementation.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O362"/>
+  <dimension ref="A1:O363"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -706,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>2935</v>
+        <v>2955</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -816,7 +816,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>59946</v>
+        <v>60208</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -871,7 +871,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>4092</v>
+        <v>3443</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1036,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>2291</v>
+        <v>2292</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>2532</v>
+        <v>2535</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -1201,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>4197</v>
+        <v>4213</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -1256,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>4525</v>
+        <v>4538</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1421,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>1372</v>
+        <v>1376</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1476,7 +1476,7 @@
         <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>1072</v>
+        <v>1516</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -1531,7 +1531,7 @@
         <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>74140</v>
+        <v>2195</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -1586,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>1080</v>
+        <v>1084</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="H22" t="n">
-        <v>11075</v>
+        <v>3268</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -1751,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>90851</v>
+        <v>91115</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -1861,7 +1861,7 @@
         <v>1</v>
       </c>
       <c r="H26" t="n">
-        <v>3638</v>
+        <v>3214</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -1971,7 +1971,7 @@
         <v>1</v>
       </c>
       <c r="H28" t="n">
-        <v>2925</v>
+        <v>2947</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
@@ -2026,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="H29" t="n">
-        <v>4666</v>
+        <v>4667</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
@@ -2136,7 +2136,7 @@
         <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>5058</v>
+        <v>5212</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
@@ -2191,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>2448</v>
+        <v>2410</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -2246,7 +2246,7 @@
         <v>1</v>
       </c>
       <c r="H33" t="n">
-        <v>6068</v>
+        <v>6138</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -2301,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="H34" t="n">
-        <v>3827</v>
+        <v>3833</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
@@ -2356,7 +2356,7 @@
         <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>3682</v>
+        <v>3685</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
@@ -2411,7 +2411,7 @@
         <v>1</v>
       </c>
       <c r="H36" t="n">
-        <v>13414</v>
+        <v>12770</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -2468,7 +2468,7 @@
         <v>1</v>
       </c>
       <c r="H37" t="n">
-        <v>361</v>
+        <v>583</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
@@ -2523,7 +2523,7 @@
         <v>1</v>
       </c>
       <c r="H38" t="n">
-        <v>4496</v>
+        <v>4498</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
@@ -2633,7 +2633,7 @@
         <v>1</v>
       </c>
       <c r="H40" t="n">
-        <v>6570</v>
+        <v>6514</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -2743,7 +2743,7 @@
         <v>1</v>
       </c>
       <c r="H42" t="n">
-        <v>2036</v>
+        <v>1878</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
@@ -2798,7 +2798,7 @@
         <v>1</v>
       </c>
       <c r="H43" t="n">
-        <v>3092</v>
+        <v>3093</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
@@ -2853,7 +2853,7 @@
         <v>1</v>
       </c>
       <c r="H44" t="n">
-        <v>5330</v>
+        <v>5337</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
@@ -2908,7 +2908,7 @@
         <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>2843</v>
+        <v>2913</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
@@ -2963,7 +2963,7 @@
         <v>1</v>
       </c>
       <c r="H46" t="n">
-        <v>5479</v>
+        <v>5481</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
@@ -3018,7 +3018,7 @@
         <v>1</v>
       </c>
       <c r="H47" t="n">
-        <v>2230</v>
+        <v>6235</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
@@ -3073,7 +3073,7 @@
         <v>1</v>
       </c>
       <c r="H48" t="n">
-        <v>5550</v>
+        <v>21305</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
@@ -3128,7 +3128,7 @@
         <v>1</v>
       </c>
       <c r="H49" t="n">
-        <v>5012</v>
+        <v>5014</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
@@ -3293,7 +3293,7 @@
         <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>23756</v>
+        <v>22487</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
@@ -3348,7 +3348,7 @@
         <v>1</v>
       </c>
       <c r="H53" t="n">
-        <v>4520</v>
+        <v>4505</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
@@ -3403,7 +3403,7 @@
         <v>1</v>
       </c>
       <c r="H54" t="n">
-        <v>4966</v>
+        <v>15596</v>
       </c>
       <c r="I54" t="n">
         <v>0</v>
@@ -3458,7 +3458,7 @@
         <v>1</v>
       </c>
       <c r="H55" t="n">
-        <v>16459</v>
+        <v>14562</v>
       </c>
       <c r="I55" t="n">
         <v>0</v>
@@ -3513,7 +3513,7 @@
         <v>1</v>
       </c>
       <c r="H56" t="n">
-        <v>10715</v>
+        <v>10718</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
@@ -3568,7 +3568,7 @@
         <v>1</v>
       </c>
       <c r="H57" t="n">
-        <v>0</v>
+        <v>33499</v>
       </c>
       <c r="I57" t="n">
         <v>12</v>
@@ -3623,7 +3623,7 @@
         <v>1</v>
       </c>
       <c r="H58" t="n">
-        <v>58</v>
+        <v>11057</v>
       </c>
       <c r="I58" t="n">
         <v>269</v>
@@ -3898,7 +3898,7 @@
         <v>1</v>
       </c>
       <c r="H63" t="n">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="I63" t="n">
         <v>0</v>
@@ -3953,7 +3953,7 @@
         <v>1</v>
       </c>
       <c r="H64" t="n">
-        <v>155048</v>
+        <v>155056</v>
       </c>
       <c r="I64" t="n">
         <v>0</v>
@@ -4008,7 +4008,7 @@
         <v>1</v>
       </c>
       <c r="H65" t="n">
-        <v>9478</v>
+        <v>9560</v>
       </c>
       <c r="I65" t="n">
         <v>0</v>
@@ -4063,7 +4063,7 @@
         <v>1</v>
       </c>
       <c r="H66" t="n">
-        <v>2155</v>
+        <v>2226</v>
       </c>
       <c r="I66" t="n">
         <v>0</v>
@@ -4173,7 +4173,7 @@
         <v>1</v>
       </c>
       <c r="H68" t="n">
-        <v>9262</v>
+        <v>8354</v>
       </c>
       <c r="I68" t="n">
         <v>0</v>
@@ -4228,7 +4228,7 @@
         <v>1</v>
       </c>
       <c r="H69" t="n">
-        <v>4155</v>
+        <v>8675</v>
       </c>
       <c r="I69" t="n">
         <v>0</v>
@@ -4338,7 +4338,7 @@
         <v>1</v>
       </c>
       <c r="H71" t="n">
-        <v>3617</v>
+        <v>3622</v>
       </c>
       <c r="I71" t="n">
         <v>0</v>
@@ -4723,7 +4723,7 @@
         <v>1</v>
       </c>
       <c r="H78" t="n">
-        <v>7016</v>
+        <v>7043</v>
       </c>
       <c r="I78" t="n">
         <v>0</v>
@@ -4778,7 +4778,7 @@
         <v>1</v>
       </c>
       <c r="H79" t="n">
-        <v>3343</v>
+        <v>3886</v>
       </c>
       <c r="I79" t="n">
         <v>0</v>
@@ -4833,7 +4833,7 @@
         <v>1</v>
       </c>
       <c r="H80" t="n">
-        <v>971</v>
+        <v>3499</v>
       </c>
       <c r="I80" t="n">
         <v>0</v>
@@ -4943,7 +4943,7 @@
         <v>1</v>
       </c>
       <c r="H82" t="n">
-        <v>12237</v>
+        <v>12287</v>
       </c>
       <c r="I82" t="n">
         <v>0</v>
@@ -5053,7 +5053,7 @@
         <v>1</v>
       </c>
       <c r="H84" t="n">
-        <v>16602</v>
+        <v>16612</v>
       </c>
       <c r="I84" t="n">
         <v>0</v>
@@ -5163,7 +5163,7 @@
         <v>1</v>
       </c>
       <c r="H86" t="n">
-        <v>2761</v>
+        <v>2785</v>
       </c>
       <c r="I86" t="n">
         <v>0</v>
@@ -5218,7 +5218,7 @@
         <v>1</v>
       </c>
       <c r="H87" t="n">
-        <v>6948</v>
+        <v>6983</v>
       </c>
       <c r="I87" t="n">
         <v>0</v>
@@ -5438,7 +5438,7 @@
         <v>1</v>
       </c>
       <c r="H91" t="n">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="I91" t="n">
         <v>0</v>
@@ -5493,7 +5493,7 @@
         <v>1</v>
       </c>
       <c r="H92" t="n">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="I92" t="n">
         <v>0</v>
@@ -5603,7 +5603,7 @@
         <v>1</v>
       </c>
       <c r="H94" t="n">
-        <v>961</v>
+        <v>978</v>
       </c>
       <c r="I94" t="n">
         <v>0</v>
@@ -5658,7 +5658,7 @@
         <v>1</v>
       </c>
       <c r="H95" t="n">
-        <v>24068</v>
+        <v>24069</v>
       </c>
       <c r="I95" t="n">
         <v>0</v>
@@ -5768,7 +5768,7 @@
         <v>1</v>
       </c>
       <c r="H97" t="n">
-        <v>5622</v>
+        <v>5642</v>
       </c>
       <c r="I97" t="n">
         <v>0</v>
@@ -6098,7 +6098,7 @@
         <v>1</v>
       </c>
       <c r="H103" t="n">
-        <v>9057</v>
+        <v>9023</v>
       </c>
       <c r="I103" t="n">
         <v>0</v>
@@ -6153,7 +6153,7 @@
         <v>1</v>
       </c>
       <c r="H104" t="n">
-        <v>3109</v>
+        <v>3121</v>
       </c>
       <c r="I104" t="n">
         <v>0</v>
@@ -6208,7 +6208,7 @@
         <v>1</v>
       </c>
       <c r="H105" t="n">
-        <v>1069</v>
+        <v>1085</v>
       </c>
       <c r="I105" t="n">
         <v>0</v>
@@ -6428,7 +6428,7 @@
         <v>1</v>
       </c>
       <c r="H109" t="n">
-        <v>587</v>
+        <v>538</v>
       </c>
       <c r="I109" t="n">
         <v>0</v>
@@ -6538,7 +6538,7 @@
         <v>1</v>
       </c>
       <c r="H111" t="n">
-        <v>4286</v>
+        <v>4290</v>
       </c>
       <c r="I111" t="n">
         <v>0</v>
@@ -6593,7 +6593,7 @@
         <v>1</v>
       </c>
       <c r="H112" t="n">
-        <v>3275</v>
+        <v>3277</v>
       </c>
       <c r="I112" t="n">
         <v>0</v>
@@ -6648,7 +6648,7 @@
         <v>1</v>
       </c>
       <c r="H113" t="n">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="I113" t="n">
         <v>0</v>
@@ -6758,7 +6758,7 @@
         <v>1</v>
       </c>
       <c r="H115" t="n">
-        <v>1284</v>
+        <v>1081</v>
       </c>
       <c r="I115" t="n">
         <v>0</v>
@@ -6813,7 +6813,7 @@
         <v>1</v>
       </c>
       <c r="H116" t="n">
-        <v>31235</v>
+        <v>31704</v>
       </c>
       <c r="I116" t="n">
         <v>0</v>
@@ -6978,7 +6978,7 @@
         <v>1</v>
       </c>
       <c r="H119" t="n">
-        <v>187</v>
+        <v>797</v>
       </c>
       <c r="I119" t="n">
         <v>0</v>
@@ -7033,7 +7033,7 @@
         <v>1</v>
       </c>
       <c r="H120" t="n">
-        <v>1255</v>
+        <v>1287</v>
       </c>
       <c r="I120" t="n">
         <v>0</v>
@@ -7088,7 +7088,7 @@
         <v>1</v>
       </c>
       <c r="H121" t="n">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="I121" t="n">
         <v>0</v>
@@ -7143,7 +7143,7 @@
         <v>1</v>
       </c>
       <c r="H122" t="n">
-        <v>8107</v>
+        <v>7941</v>
       </c>
       <c r="I122" t="n">
         <v>0</v>
@@ -7198,7 +7198,7 @@
         <v>1</v>
       </c>
       <c r="H123" t="n">
-        <v>2841</v>
+        <v>2837</v>
       </c>
       <c r="I123" t="n">
         <v>0</v>
@@ -7253,7 +7253,7 @@
         <v>1</v>
       </c>
       <c r="H124" t="n">
-        <v>8522</v>
+        <v>4920</v>
       </c>
       <c r="I124" t="n">
         <v>0</v>
@@ -7308,7 +7308,7 @@
         <v>1</v>
       </c>
       <c r="H125" t="n">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="I125" t="n">
         <v>0</v>
@@ -7363,7 +7363,7 @@
         <v>1</v>
       </c>
       <c r="H126" t="n">
-        <v>1305</v>
+        <v>1274</v>
       </c>
       <c r="I126" t="n">
         <v>0</v>
@@ -7418,7 +7418,7 @@
         <v>1</v>
       </c>
       <c r="H127" t="n">
-        <v>984</v>
+        <v>977</v>
       </c>
       <c r="I127" t="n">
         <v>0</v>
@@ -7473,7 +7473,7 @@
         <v>1</v>
       </c>
       <c r="H128" t="n">
-        <v>4051</v>
+        <v>4062</v>
       </c>
       <c r="I128" t="n">
         <v>0</v>
@@ -7528,7 +7528,7 @@
         <v>1</v>
       </c>
       <c r="H129" t="n">
-        <v>15304</v>
+        <v>15358</v>
       </c>
       <c r="I129" t="n">
         <v>0</v>
@@ -7583,7 +7583,7 @@
         <v>1</v>
       </c>
       <c r="H130" t="n">
-        <v>21198</v>
+        <v>21197</v>
       </c>
       <c r="I130" t="n">
         <v>0</v>
@@ -7638,7 +7638,7 @@
         <v>1</v>
       </c>
       <c r="H131" t="n">
-        <v>1358</v>
+        <v>1368</v>
       </c>
       <c r="I131" t="n">
         <v>0</v>
@@ -7693,7 +7693,7 @@
         <v>1</v>
       </c>
       <c r="H132" t="n">
-        <v>1104</v>
+        <v>1118</v>
       </c>
       <c r="I132" t="n">
         <v>0</v>
@@ -7748,7 +7748,7 @@
         <v>1</v>
       </c>
       <c r="H133" t="n">
-        <v>4</v>
+        <v>608</v>
       </c>
       <c r="I133" t="n">
         <v>0</v>
@@ -7803,7 +7803,7 @@
         <v>1</v>
       </c>
       <c r="H134" t="n">
-        <v>18398</v>
+        <v>18421</v>
       </c>
       <c r="I134" t="n">
         <v>0</v>
@@ -7858,7 +7858,7 @@
         <v>1</v>
       </c>
       <c r="H135" t="n">
-        <v>15406</v>
+        <v>17397</v>
       </c>
       <c r="I135" t="n">
         <v>0</v>
@@ -7913,7 +7913,7 @@
         <v>1</v>
       </c>
       <c r="H136" t="n">
-        <v>4673</v>
+        <v>4705</v>
       </c>
       <c r="I136" t="n">
         <v>0</v>
@@ -7968,7 +7968,7 @@
         <v>1</v>
       </c>
       <c r="H137" t="n">
-        <v>1055</v>
+        <v>1071</v>
       </c>
       <c r="I137" t="n">
         <v>0</v>
@@ -8188,7 +8188,7 @@
         <v>1</v>
       </c>
       <c r="H141" t="n">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="I141" t="n">
         <v>0</v>
@@ -8298,7 +8298,7 @@
         <v>1</v>
       </c>
       <c r="H143" t="n">
-        <v>928</v>
+        <v>931</v>
       </c>
       <c r="I143" t="n">
         <v>0</v>
@@ -8353,7 +8353,7 @@
         <v>1</v>
       </c>
       <c r="H144" t="n">
-        <v>3862</v>
+        <v>3891</v>
       </c>
       <c r="I144" t="n">
         <v>0</v>
@@ -8408,7 +8408,7 @@
         <v>1</v>
       </c>
       <c r="H145" t="n">
-        <v>2781</v>
+        <v>2423</v>
       </c>
       <c r="I145" t="n">
         <v>0</v>
@@ -8738,7 +8738,7 @@
         <v>1</v>
       </c>
       <c r="H151" t="n">
-        <v>88685</v>
+        <v>89712</v>
       </c>
       <c r="I151" t="n">
         <v>0</v>
@@ -8903,7 +8903,7 @@
         <v>1</v>
       </c>
       <c r="H154" t="n">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="I154" t="n">
         <v>0</v>
@@ -8958,7 +8958,7 @@
         <v>1</v>
       </c>
       <c r="H155" t="n">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="I155" t="n">
         <v>0</v>
@@ -9013,7 +9013,7 @@
         <v>1</v>
       </c>
       <c r="H156" t="n">
-        <v>10072</v>
+        <v>10104</v>
       </c>
       <c r="I156" t="n">
         <v>9</v>
@@ -9068,7 +9068,7 @@
         <v>1</v>
       </c>
       <c r="H157" t="n">
-        <v>2086</v>
+        <v>2097</v>
       </c>
       <c r="I157" t="n">
         <v>0</v>
@@ -9123,7 +9123,7 @@
         <v>1</v>
       </c>
       <c r="H158" t="n">
-        <v>806</v>
+        <v>815</v>
       </c>
       <c r="I158" t="n">
         <v>0</v>
@@ -9233,7 +9233,7 @@
         <v>1</v>
       </c>
       <c r="H160" t="n">
-        <v>12417</v>
+        <v>12452</v>
       </c>
       <c r="I160" t="n">
         <v>0</v>
@@ -9288,7 +9288,7 @@
         <v>1</v>
       </c>
       <c r="H161" t="n">
-        <v>1502</v>
+        <v>1546</v>
       </c>
       <c r="I161" t="n">
         <v>0</v>
@@ -9508,7 +9508,7 @@
         <v>1</v>
       </c>
       <c r="H165" t="n">
-        <v>4452</v>
+        <v>4453</v>
       </c>
       <c r="I165" t="n">
         <v>0</v>
@@ -9563,7 +9563,7 @@
         <v>1</v>
       </c>
       <c r="H166" t="n">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="I166" t="n">
         <v>0</v>
@@ -9620,7 +9620,7 @@
         <v>1</v>
       </c>
       <c r="H167" t="n">
-        <v>2335</v>
+        <v>2344</v>
       </c>
       <c r="I167" t="n">
         <v>0</v>
@@ -9675,7 +9675,7 @@
         <v>1</v>
       </c>
       <c r="H168" t="n">
-        <v>1627</v>
+        <v>1629</v>
       </c>
       <c r="I168" t="n">
         <v>0</v>
@@ -9730,7 +9730,7 @@
         <v>1</v>
       </c>
       <c r="H169" t="n">
-        <v>2984</v>
+        <v>2986</v>
       </c>
       <c r="I169" t="n">
         <v>0</v>
@@ -9950,7 +9950,7 @@
         <v>1</v>
       </c>
       <c r="H173" t="n">
-        <v>7769</v>
+        <v>7799</v>
       </c>
       <c r="I173" t="n">
         <v>0</v>
@@ -10060,7 +10060,7 @@
         <v>1</v>
       </c>
       <c r="H175" t="n">
-        <v>3337</v>
+        <v>3347</v>
       </c>
       <c r="I175" t="n">
         <v>6</v>
@@ -10170,7 +10170,7 @@
         <v>1</v>
       </c>
       <c r="H177" t="n">
-        <v>256</v>
+        <v>148</v>
       </c>
       <c r="I177" t="n">
         <v>0</v>
@@ -10225,7 +10225,7 @@
         <v>1</v>
       </c>
       <c r="H178" t="n">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="I178" t="n">
         <v>0</v>
@@ -10445,7 +10445,7 @@
         <v>1</v>
       </c>
       <c r="H182" t="n">
-        <v>2582</v>
+        <v>2585</v>
       </c>
       <c r="I182" t="n">
         <v>0</v>
@@ -10720,7 +10720,7 @@
         <v>1</v>
       </c>
       <c r="H187" t="n">
-        <v>12453</v>
+        <v>12442</v>
       </c>
       <c r="I187" t="n">
         <v>0</v>
@@ -10775,7 +10775,7 @@
         <v>1</v>
       </c>
       <c r="H188" t="n">
-        <v>1351</v>
+        <v>1342</v>
       </c>
       <c r="I188" t="n">
         <v>0</v>
@@ -10830,7 +10830,7 @@
         <v>1</v>
       </c>
       <c r="H189" t="n">
-        <v>31608</v>
+        <v>31764</v>
       </c>
       <c r="I189" t="n">
         <v>0</v>
@@ -10940,7 +10940,7 @@
         <v>1</v>
       </c>
       <c r="H191" t="n">
-        <v>5054</v>
+        <v>5079</v>
       </c>
       <c r="I191" t="n">
         <v>0</v>
@@ -11160,7 +11160,7 @@
         <v>1</v>
       </c>
       <c r="H195" t="n">
-        <v>1554</v>
+        <v>1574</v>
       </c>
       <c r="I195" t="n">
         <v>0</v>
@@ -11270,7 +11270,7 @@
         <v>1</v>
       </c>
       <c r="H197" t="n">
-        <v>959</v>
+        <v>963</v>
       </c>
       <c r="I197" t="n">
         <v>0</v>
@@ -11435,7 +11435,7 @@
         <v>1</v>
       </c>
       <c r="H200" t="n">
-        <v>1893</v>
+        <v>1906</v>
       </c>
       <c r="I200" t="n">
         <v>0</v>
@@ -11490,7 +11490,7 @@
         <v>1</v>
       </c>
       <c r="H201" t="n">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="I201" t="n">
         <v>0</v>
@@ -11600,7 +11600,7 @@
         <v>1</v>
       </c>
       <c r="H203" t="n">
-        <v>9771</v>
+        <v>9808</v>
       </c>
       <c r="I203" t="n">
         <v>0</v>
@@ -11657,7 +11657,7 @@
         <v>1</v>
       </c>
       <c r="H204" t="n">
-        <v>4973</v>
+        <v>4975</v>
       </c>
       <c r="I204" t="n">
         <v>0</v>
@@ -11712,7 +11712,7 @@
         <v>1</v>
       </c>
       <c r="H205" t="n">
-        <v>2056</v>
+        <v>2052</v>
       </c>
       <c r="I205" t="n">
         <v>0</v>
@@ -11932,7 +11932,7 @@
         <v>1</v>
       </c>
       <c r="H209" t="n">
-        <v>3647</v>
+        <v>3705</v>
       </c>
       <c r="I209" t="n">
         <v>0</v>
@@ -11987,7 +11987,7 @@
         <v>1</v>
       </c>
       <c r="H210" t="n">
-        <v>3654</v>
+        <v>3655</v>
       </c>
       <c r="I210" t="n">
         <v>0</v>
@@ -12317,7 +12317,7 @@
         <v>1</v>
       </c>
       <c r="H216" t="n">
-        <v>4204</v>
+        <v>4205</v>
       </c>
       <c r="I216" t="n">
         <v>0</v>
@@ -12372,7 +12372,7 @@
         <v>1</v>
       </c>
       <c r="H217" t="n">
-        <v>1464</v>
+        <v>1466</v>
       </c>
       <c r="I217" t="n">
         <v>0</v>
@@ -12427,7 +12427,7 @@
         <v>1</v>
       </c>
       <c r="H218" t="n">
-        <v>3322</v>
+        <v>3316</v>
       </c>
       <c r="I218" t="n">
         <v>0</v>
@@ -12537,7 +12537,7 @@
         <v>1</v>
       </c>
       <c r="H220" t="n">
-        <v>8564</v>
+        <v>8658</v>
       </c>
       <c r="I220" t="n">
         <v>0</v>
@@ -12702,7 +12702,7 @@
         <v>1</v>
       </c>
       <c r="H223" t="n">
-        <v>36979</v>
+        <v>36993</v>
       </c>
       <c r="I223" t="n">
         <v>0</v>
@@ -12757,7 +12757,7 @@
         <v>1</v>
       </c>
       <c r="H224" t="n">
-        <v>1668</v>
+        <v>1670</v>
       </c>
       <c r="I224" t="n">
         <v>0</v>
@@ -12812,7 +12812,7 @@
         <v>1</v>
       </c>
       <c r="H225" t="n">
-        <v>3945</v>
+        <v>3942</v>
       </c>
       <c r="I225" t="n">
         <v>0</v>
@@ -12867,7 +12867,7 @@
         <v>1</v>
       </c>
       <c r="H226" t="n">
-        <v>3818</v>
+        <v>3903</v>
       </c>
       <c r="I226" t="n">
         <v>0</v>
@@ -12977,7 +12977,7 @@
         <v>1</v>
       </c>
       <c r="H228" t="n">
-        <v>1463</v>
+        <v>1468</v>
       </c>
       <c r="I228" t="n">
         <v>4</v>
@@ -13032,7 +13032,7 @@
         <v>1</v>
       </c>
       <c r="H229" t="n">
-        <v>7923</v>
+        <v>7963</v>
       </c>
       <c r="I229" t="n">
         <v>0</v>
@@ -13087,7 +13087,7 @@
         <v>1</v>
       </c>
       <c r="H230" t="n">
-        <v>2728</v>
+        <v>3083</v>
       </c>
       <c r="I230" t="n">
         <v>0</v>
@@ -13252,7 +13252,7 @@
         <v>1</v>
       </c>
       <c r="H233" t="n">
-        <v>1100</v>
+        <v>1103</v>
       </c>
       <c r="I233" t="n">
         <v>0</v>
@@ -13307,7 +13307,7 @@
         <v>1</v>
       </c>
       <c r="H234" t="n">
-        <v>4037</v>
+        <v>4051</v>
       </c>
       <c r="I234" t="n">
         <v>0</v>
@@ -13417,7 +13417,7 @@
         <v>1</v>
       </c>
       <c r="H236" t="n">
-        <v>920</v>
+        <v>3598</v>
       </c>
       <c r="I236" t="n">
         <v>0</v>
@@ -13527,7 +13527,7 @@
         <v>1</v>
       </c>
       <c r="H238" t="n">
-        <v>1707</v>
+        <v>1668</v>
       </c>
       <c r="I238" t="n">
         <v>0</v>
@@ -13637,7 +13637,7 @@
         <v>1</v>
       </c>
       <c r="H240" t="n">
-        <v>20857</v>
+        <v>20870</v>
       </c>
       <c r="I240" t="n">
         <v>0</v>
@@ -13747,7 +13747,7 @@
         <v>1</v>
       </c>
       <c r="H242" t="n">
-        <v>1297</v>
+        <v>1357</v>
       </c>
       <c r="I242" t="n">
         <v>0</v>
@@ -13802,7 +13802,7 @@
         <v>1</v>
       </c>
       <c r="H243" t="n">
-        <v>1760</v>
+        <v>4793</v>
       </c>
       <c r="I243" t="n">
         <v>0</v>
@@ -13857,7 +13857,7 @@
         <v>1</v>
       </c>
       <c r="H244" t="n">
-        <v>159552</v>
+        <v>1582</v>
       </c>
       <c r="I244" t="n">
         <v>0</v>
@@ -13912,7 +13912,7 @@
         <v>1</v>
       </c>
       <c r="H245" t="n">
-        <v>3580</v>
+        <v>3404</v>
       </c>
       <c r="I245" t="n">
         <v>0</v>
@@ -13967,7 +13967,7 @@
         <v>1</v>
       </c>
       <c r="H246" t="n">
-        <v>1337</v>
+        <v>1339</v>
       </c>
       <c r="I246" t="n">
         <v>0</v>
@@ -14022,7 +14022,7 @@
         <v>1</v>
       </c>
       <c r="H247" t="n">
-        <v>2581</v>
+        <v>2589</v>
       </c>
       <c r="I247" t="n">
         <v>0</v>
@@ -14242,7 +14242,7 @@
         <v>1</v>
       </c>
       <c r="H251" t="n">
-        <v>48902</v>
+        <v>50432</v>
       </c>
       <c r="I251" t="n">
         <v>0</v>
@@ -14352,7 +14352,7 @@
         <v>1</v>
       </c>
       <c r="H253" t="n">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="I253" t="n">
         <v>0</v>
@@ -14407,7 +14407,7 @@
         <v>1</v>
       </c>
       <c r="H254" t="n">
-        <v>2211</v>
+        <v>2217</v>
       </c>
       <c r="I254" t="n">
         <v>0</v>
@@ -14517,7 +14517,7 @@
         <v>1</v>
       </c>
       <c r="H256" t="n">
-        <v>4019</v>
+        <v>4068</v>
       </c>
       <c r="I256" t="n">
         <v>0</v>
@@ -14572,7 +14572,7 @@
         <v>1</v>
       </c>
       <c r="H257" t="n">
-        <v>479</v>
+        <v>437</v>
       </c>
       <c r="I257" t="n">
         <v>0</v>
@@ -14737,7 +14737,7 @@
         <v>1</v>
       </c>
       <c r="H260" t="n">
-        <v>1623</v>
+        <v>1759</v>
       </c>
       <c r="I260" t="n">
         <v>0</v>
@@ -14792,7 +14792,7 @@
         <v>1</v>
       </c>
       <c r="H261" t="n">
-        <v>0</v>
+        <v>16619</v>
       </c>
       <c r="I261" t="n">
         <v>0</v>
@@ -14902,7 +14902,7 @@
         <v>1</v>
       </c>
       <c r="H263" t="n">
-        <v>6615</v>
+        <v>632</v>
       </c>
       <c r="I263" t="n">
         <v>0</v>
@@ -14957,7 +14957,7 @@
         <v>1</v>
       </c>
       <c r="H264" t="n">
-        <v>7608</v>
+        <v>7656</v>
       </c>
       <c r="I264" t="n">
         <v>0</v>
@@ -15067,7 +15067,7 @@
         <v>1</v>
       </c>
       <c r="H266" t="n">
-        <v>46041</v>
+        <v>1029</v>
       </c>
       <c r="I266" t="n">
         <v>0</v>
@@ -15124,7 +15124,7 @@
         <v>1</v>
       </c>
       <c r="H267" t="n">
-        <v>10566</v>
+        <v>10561</v>
       </c>
       <c r="I267" t="n">
         <v>0</v>
@@ -15179,7 +15179,7 @@
         <v>1</v>
       </c>
       <c r="H268" t="n">
-        <v>3129</v>
+        <v>3126</v>
       </c>
       <c r="I268" t="n">
         <v>0</v>
@@ -15344,7 +15344,7 @@
         <v>1</v>
       </c>
       <c r="H271" t="n">
-        <v>4715</v>
+        <v>4714</v>
       </c>
       <c r="I271" t="n">
         <v>0</v>
@@ -15399,7 +15399,7 @@
         <v>1</v>
       </c>
       <c r="H272" t="n">
-        <v>4902</v>
+        <v>4909</v>
       </c>
       <c r="I272" t="n">
         <v>0</v>
@@ -15509,7 +15509,7 @@
         <v>1</v>
       </c>
       <c r="H274" t="n">
-        <v>11936</v>
+        <v>11954</v>
       </c>
       <c r="I274" t="n">
         <v>0</v>
@@ -15564,7 +15564,7 @@
         <v>1</v>
       </c>
       <c r="H275" t="n">
-        <v>7994</v>
+        <v>7996</v>
       </c>
       <c r="I275" t="n">
         <v>0</v>
@@ -15676,7 +15676,7 @@
         <v>1</v>
       </c>
       <c r="H277" t="n">
-        <v>1020</v>
+        <v>1009</v>
       </c>
       <c r="I277" t="n">
         <v>0</v>
@@ -15841,7 +15841,7 @@
         <v>1</v>
       </c>
       <c r="H280" t="n">
-        <v>1637</v>
+        <v>1642</v>
       </c>
       <c r="I280" t="n">
         <v>0</v>
@@ -15951,7 +15951,7 @@
         <v>1</v>
       </c>
       <c r="H282" t="n">
-        <v>24479</v>
+        <v>24653</v>
       </c>
       <c r="I282" t="n">
         <v>0</v>
@@ -16061,7 +16061,7 @@
         <v>1</v>
       </c>
       <c r="H284" t="n">
-        <v>4397</v>
+        <v>4464</v>
       </c>
       <c r="I284" t="n">
         <v>0</v>
@@ -16281,7 +16281,7 @@
         <v>1</v>
       </c>
       <c r="H288" t="n">
-        <v>1507</v>
+        <v>1528</v>
       </c>
       <c r="I288" t="n">
         <v>0</v>
@@ -16336,7 +16336,7 @@
         <v>1</v>
       </c>
       <c r="H289" t="n">
-        <v>665</v>
+        <v>696</v>
       </c>
       <c r="I289" t="n">
         <v>0</v>
@@ -16391,7 +16391,7 @@
         <v>1</v>
       </c>
       <c r="H290" t="n">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I290" t="n">
         <v>0</v>
@@ -16501,7 +16501,7 @@
         <v>1</v>
       </c>
       <c r="H292" t="n">
-        <v>1664</v>
+        <v>1712</v>
       </c>
       <c r="I292" t="n">
         <v>0</v>
@@ -16556,7 +16556,7 @@
         <v>1</v>
       </c>
       <c r="H293" t="n">
-        <v>2860</v>
+        <v>2924</v>
       </c>
       <c r="I293" t="n">
         <v>0</v>
@@ -16776,7 +16776,7 @@
         <v>1</v>
       </c>
       <c r="H297" t="n">
-        <v>0</v>
+        <v>447</v>
       </c>
       <c r="I297" t="n">
         <v>0</v>
@@ -16886,7 +16886,7 @@
         <v>1</v>
       </c>
       <c r="H299" t="n">
-        <v>8262</v>
+        <v>8265</v>
       </c>
       <c r="I299" t="n">
         <v>0</v>
@@ -16941,7 +16941,7 @@
         <v>1</v>
       </c>
       <c r="H300" t="n">
-        <v>2706</v>
+        <v>2716</v>
       </c>
       <c r="I300" t="n">
         <v>0</v>
@@ -17051,7 +17051,7 @@
         <v>1</v>
       </c>
       <c r="H302" t="n">
-        <v>1258</v>
+        <v>1262</v>
       </c>
       <c r="I302" t="n">
         <v>0</v>
@@ -17106,7 +17106,7 @@
         <v>1</v>
       </c>
       <c r="H303" t="n">
-        <v>5795</v>
+        <v>5794</v>
       </c>
       <c r="I303" t="n">
         <v>0</v>
@@ -17161,7 +17161,7 @@
         <v>1</v>
       </c>
       <c r="H304" t="n">
-        <v>911</v>
+        <v>1199</v>
       </c>
       <c r="I304" t="n">
         <v>0</v>
@@ -17216,7 +17216,7 @@
         <v>1</v>
       </c>
       <c r="H305" t="n">
-        <v>7375</v>
+        <v>7757</v>
       </c>
       <c r="I305" t="n">
         <v>0</v>
@@ -17326,7 +17326,7 @@
         <v>1</v>
       </c>
       <c r="H307" t="n">
-        <v>2126</v>
+        <v>2145</v>
       </c>
       <c r="I307" t="n">
         <v>0</v>
@@ -17491,7 +17491,7 @@
         <v>1</v>
       </c>
       <c r="H310" t="n">
-        <v>11166</v>
+        <v>11222</v>
       </c>
       <c r="I310" t="n">
         <v>0</v>
@@ -17546,7 +17546,7 @@
         <v>1</v>
       </c>
       <c r="H311" t="n">
-        <v>4128</v>
+        <v>4129</v>
       </c>
       <c r="I311" t="n">
         <v>0</v>
@@ -17656,7 +17656,7 @@
         <v>1</v>
       </c>
       <c r="H313" t="n">
-        <v>5599</v>
+        <v>1295</v>
       </c>
       <c r="I313" t="n">
         <v>0</v>
@@ -17711,7 +17711,7 @@
         <v>1</v>
       </c>
       <c r="H314" t="n">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="I314" t="n">
         <v>0</v>
@@ -17766,7 +17766,7 @@
         <v>1</v>
       </c>
       <c r="H315" t="n">
-        <v>3654</v>
+        <v>3701</v>
       </c>
       <c r="I315" t="n">
         <v>0</v>
@@ -17821,7 +17821,7 @@
         <v>1</v>
       </c>
       <c r="H316" t="n">
-        <v>840</v>
+        <v>849</v>
       </c>
       <c r="I316" t="n">
         <v>0</v>
@@ -17876,7 +17876,7 @@
         <v>1</v>
       </c>
       <c r="H317" t="n">
-        <v>811</v>
+        <v>816</v>
       </c>
       <c r="I317" t="n">
         <v>0</v>
@@ -17931,7 +17931,7 @@
         <v>1</v>
       </c>
       <c r="H318" t="n">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="I318" t="n">
         <v>0</v>
@@ -18096,7 +18096,7 @@
         <v>1</v>
       </c>
       <c r="H321" t="n">
-        <v>697</v>
+        <v>741</v>
       </c>
       <c r="I321" t="n">
         <v>0</v>
@@ -18151,7 +18151,7 @@
         <v>1</v>
       </c>
       <c r="H322" t="n">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="I322" t="n">
         <v>0</v>
@@ -18206,7 +18206,7 @@
         <v>1</v>
       </c>
       <c r="H323" t="n">
-        <v>2456</v>
+        <v>2468</v>
       </c>
       <c r="I323" t="n">
         <v>0</v>
@@ -18261,7 +18261,7 @@
         <v>1</v>
       </c>
       <c r="H324" t="n">
-        <v>4322</v>
+        <v>4677</v>
       </c>
       <c r="I324" t="n">
         <v>0</v>
@@ -18371,7 +18371,7 @@
         <v>1</v>
       </c>
       <c r="H326" t="n">
-        <v>10161</v>
+        <v>10196</v>
       </c>
       <c r="I326" t="n">
         <v>27</v>
@@ -18426,7 +18426,7 @@
         <v>1</v>
       </c>
       <c r="H327" t="n">
-        <v>2989</v>
+        <v>3008</v>
       </c>
       <c r="I327" t="n">
         <v>0</v>
@@ -18481,7 +18481,7 @@
         <v>1</v>
       </c>
       <c r="H328" t="n">
-        <v>3006</v>
+        <v>3003</v>
       </c>
       <c r="I328" t="n">
         <v>0</v>
@@ -18536,7 +18536,7 @@
         <v>1</v>
       </c>
       <c r="H329" t="n">
-        <v>2649</v>
+        <v>2678</v>
       </c>
       <c r="I329" t="n">
         <v>0</v>
@@ -18591,7 +18591,7 @@
         <v>1</v>
       </c>
       <c r="H330" t="n">
-        <v>1121</v>
+        <v>1138</v>
       </c>
       <c r="I330" t="n">
         <v>0</v>
@@ -18701,7 +18701,7 @@
         <v>1</v>
       </c>
       <c r="H332" t="n">
-        <v>206</v>
+        <v>2868</v>
       </c>
       <c r="I332" t="n">
         <v>0</v>
@@ -18756,7 +18756,7 @@
         <v>1</v>
       </c>
       <c r="H333" t="n">
-        <v>3149</v>
+        <v>3137</v>
       </c>
       <c r="I333" t="n">
         <v>0</v>
@@ -18811,7 +18811,7 @@
         <v>1</v>
       </c>
       <c r="H334" t="n">
-        <v>7399</v>
+        <v>7410</v>
       </c>
       <c r="I334" t="n">
         <v>9</v>
@@ -18866,7 +18866,7 @@
         <v>1</v>
       </c>
       <c r="H335" t="n">
-        <v>1335</v>
+        <v>1339</v>
       </c>
       <c r="I335" t="n">
         <v>0</v>
@@ -18921,7 +18921,7 @@
         <v>1</v>
       </c>
       <c r="H336" t="n">
-        <v>5000</v>
+        <v>5014</v>
       </c>
       <c r="I336" t="n">
         <v>0</v>
@@ -18976,7 +18976,7 @@
         <v>1</v>
       </c>
       <c r="H337" t="n">
-        <v>8162</v>
+        <v>8172</v>
       </c>
       <c r="I337" t="n">
         <v>0</v>
@@ -19031,7 +19031,7 @@
         <v>1</v>
       </c>
       <c r="H338" t="n">
-        <v>5328</v>
+        <v>5327</v>
       </c>
       <c r="I338" t="n">
         <v>0</v>
@@ -19086,7 +19086,7 @@
         <v>1</v>
       </c>
       <c r="H339" t="n">
-        <v>1515</v>
+        <v>1517</v>
       </c>
       <c r="I339" t="n">
         <v>0</v>
@@ -19141,7 +19141,7 @@
         <v>1</v>
       </c>
       <c r="H340" t="n">
-        <v>14740</v>
+        <v>14724</v>
       </c>
       <c r="I340" t="n">
         <v>0</v>
@@ -19196,7 +19196,7 @@
         <v>1</v>
       </c>
       <c r="H341" t="n">
-        <v>1418</v>
+        <v>1444</v>
       </c>
       <c r="I341" t="n">
         <v>0</v>
@@ -19416,7 +19416,7 @@
         <v>1</v>
       </c>
       <c r="H345" t="n">
-        <v>1542</v>
+        <v>1551</v>
       </c>
       <c r="I345" t="n">
         <v>0</v>
@@ -19471,7 +19471,7 @@
         <v>1</v>
       </c>
       <c r="H346" t="n">
-        <v>2473</v>
+        <v>2462</v>
       </c>
       <c r="I346" t="n">
         <v>0</v>
@@ -19636,7 +19636,7 @@
         <v>1</v>
       </c>
       <c r="H349" t="n">
-        <v>333</v>
+        <v>289</v>
       </c>
       <c r="I349" t="n">
         <v>0</v>
@@ -19746,7 +19746,7 @@
         <v>1</v>
       </c>
       <c r="H351" t="n">
-        <v>22007</v>
+        <v>22073</v>
       </c>
       <c r="I351" t="n">
         <v>0</v>
@@ -20021,7 +20021,7 @@
         <v>1</v>
       </c>
       <c r="H356" t="n">
-        <v>13415</v>
+        <v>13495</v>
       </c>
       <c r="I356" t="n">
         <v>0</v>
@@ -20076,7 +20076,7 @@
         <v>1</v>
       </c>
       <c r="H357" t="n">
-        <v>2849</v>
+        <v>2921</v>
       </c>
       <c r="I357" t="n">
         <v>0</v>
@@ -20375,7 +20375,62 @@
         <v>5</v>
       </c>
     </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>liferay</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>liferay-portal</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>Enterprise Resource Planning</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>38220df7f113ab58af84b3297d81db6bb40d3320</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr"/>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>2024-10-12 00:30:11+00:00</t>
+        </is>
+      </c>
+      <c r="G363" t="b">
+        <v>1</v>
+      </c>
+      <c r="H363" t="n">
+        <v>109041</v>
+      </c>
+      <c r="I363" t="n">
+        <v>0</v>
+      </c>
+      <c r="J363" t="n">
+        <v>0</v>
+      </c>
+      <c r="K363" t="n">
+        <v>32</v>
+      </c>
+      <c r="L363" t="n">
+        <v>215</v>
+      </c>
+      <c r="M363" t="n">
+        <v>155</v>
+      </c>
+      <c r="N363" t="n">
+        <v>1</v>
+      </c>
+      <c r="O363" t="n">
+        <v>1332</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>